<commit_message>
finalized schedule and added a calendar page/link to navbar
</commit_message>
<xml_diff>
--- a/schedule_130.xlsx
+++ b/schedule_130.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>date</t>
   </si>
@@ -53,88 +53,107 @@
     <t>Exploratory Data Analysis</t>
   </si>
   <si>
-    <t>Lab 1 (Due 8/27)</t>
-  </si>
-  <si>
-    <t>Lab 2 (Due 9/3)</t>
-  </si>
-  <si>
-    <t>Lab 3 (Due 9/10)</t>
-  </si>
-  <si>
-    <t>Lab 4 (Due 9/10)</t>
-  </si>
-  <si>
-    <t>Peer Eval Due (9/25)</t>
-  </si>
-  <si>
-    <t>Data Camp (Due 8/24)</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
-    <t>Proposal Due 9/19 
-* Report Due (9/22)</t>
-  </si>
-  <si>
-    <t>Install Programs [Instruction slides]() 
-* Create Data Camp Account &amp; join class (Use emailed link!)</t>
-  </si>
-  <si>
     <t>Open work on EDA</t>
   </si>
   <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
     <t>Read the EDA Instructions</t>
   </si>
   <si>
-    <t>Control your Factors</t>
+    <t>Data Camp: Intro to R - Basics module 1 due by end of class</t>
+  </si>
+  <si>
+    <t>Lab 1</t>
+  </si>
+  <si>
+    <t>Lab 2</t>
+  </si>
+  <si>
+    <t>Lab 3</t>
+  </si>
+  <si>
+    <t>Lab 4</t>
+  </si>
+  <si>
+    <t>Proposal * Report</t>
+  </si>
+  <si>
+    <t>Peer Evaluation</t>
+  </si>
+  <si>
+    <t>Read Lab 2 overview</t>
+  </si>
+  <si>
+    <t>Importing Data into R  
+* Factors
+* Functions</t>
+  </si>
+  <si>
+    <t>Data Visualizations for univariate and bivariate relationships</t>
+  </si>
+  <si>
+    <t>Multivariate and advanced data visualizations</t>
+  </si>
+  <si>
+    <t>Data cleaning and aggregation</t>
+  </si>
+  <si>
+    <t>Read Lab 4 overview</t>
+  </si>
+  <si>
+    <t>packages needed: tidyverse, rmarkdown, knitr, kable, kableExtra, gridExtra</t>
+  </si>
+  <si>
+    <t>paneling and gridExtra</t>
+  </si>
+  <si>
+    <t>ggplot, kable tables</t>
+  </si>
+  <si>
+    <t>dplyr</t>
+  </si>
+  <si>
+    <t>Combining data from multiple sources</t>
+  </si>
+  <si>
+    <t>dplyr joins</t>
+  </si>
+  <si>
+    <t>Functions for Statistical Analyses</t>
+  </si>
+  <si>
+    <t>R Studio suite of awesomeness
+* R packages - how things get done
+* Reproducible Research with R Markdown</t>
+  </si>
+  <si>
+    <t>Install programs on your personal computer [SlideDeck]()
+* Read Lab 1 overview</t>
+  </si>
+  <si>
+    <t>Create Data Camp Account &amp; join class (Use emailed link!)</t>
+  </si>
+  <si>
+    <t>Read Lab 5 overview</t>
+  </si>
+  <si>
+    <t>Lab 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baseball data? </t>
   </si>
   <si>
     <t>Logistics 
-* Accounts
-* Intro to R</t>
-  </si>
-  <si>
-    <t>Read Lab 2 instructions</t>
-  </si>
-  <si>
-    <t>Data Camp - Intro to R (Entire Module)
-* Read lab 1 instructions</t>
-  </si>
-  <si>
-    <t>Read Lab 3 instructions
-* install the `ggplot2` package</t>
-  </si>
-  <si>
-    <t>R packages - How R works
-* R Studio suite of awesomeness
-* Reproducible Research with R Markdown</t>
-  </si>
-  <si>
-    <t>Get that data into R  
-* Missing Data
-* Functions</t>
-  </si>
-  <si>
-    <t>Data Manipulation and Aggregation
-* tidy data</t>
-  </si>
-  <si>
-    <t>Read Lab 4 instructions
-* install the `dplyr` package</t>
-  </si>
-  <si>
-    <t>Functions for Statistical Analysis</t>
+* Intro to R using Data Camp
+* How to get help</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -320,7 +339,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,9 +392,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -388,27 +404,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -427,9 +431,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -441,6 +442,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -840,26 +874,26 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="1"/>
-    <col min="3" max="3" width="4.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.08203125" style="29" customWidth="1"/>
     <col min="7" max="7" width="23.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.625" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.875" style="1"/>
+    <col min="8" max="8" width="29.58203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -867,27 +901,27 @@
       <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="36" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="26" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="38" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="19"/>
+      <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -898,20 +932,20 @@
         <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="20"/>
+      <c r="D2" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="39"/>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
         <f>B2+2</f>
@@ -921,20 +955,22 @@
         <f>TEXT(WEEKDAY(B3,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="38" t="s">
-        <v>24</v>
+      <c r="D3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="32" t="s">
+        <v>33</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="21"/>
+        <v>13</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>25</v>
+      </c>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -947,20 +983,20 @@
         <f>TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="34" t="s">
-        <v>23</v>
+      <c r="D4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="29" t="s">
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="22"/>
+        <v>14</v>
+      </c>
+      <c r="H4" s="39"/>
+      <c r="I4" s="21"/>
     </row>
-    <row r="5" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="5">
         <f>B4+2</f>
@@ -970,20 +1006,18 @@
         <f>TEXT(WEEKDAY(B5,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="38" t="s">
-        <v>25</v>
-      </c>
+      <c r="D5" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="23"/>
+        <v>15</v>
+      </c>
+      <c r="H5" s="41"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f>A4+1</f>
         <v>3</v>
@@ -996,14 +1030,22 @@
         <f t="shared" ref="C6:C11" si="0">TEXT(WEEKDAY(B6,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="24"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="5">
         <f>B6+2</f>
@@ -1013,14 +1055,18 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="35"/>
+      <c r="D7" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="25"/>
+      <c r="H7" s="42" t="s">
+        <v>26</v>
+      </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" ref="A8:A10" si="1">A6+1</f>
         <v>4</v>
@@ -1033,19 +1079,21 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="10"/>
       <c r="B9" s="11">
         <f>B8+2</f>
@@ -1056,16 +1104,18 @@
         <v>Thu</v>
       </c>
       <c r="D9" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="29"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="22"/>
+      <c r="J9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1078,20 +1128,22 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="39" t="s">
-        <v>20</v>
+      <c r="E10" s="23"/>
+      <c r="F10" s="33" t="s">
+        <v>11</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="27"/>
+        <v>17</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>37</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5">
         <f>B10+2</f>
@@ -1101,15 +1153,15 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="41"/>
       <c r="I11" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor adjustments to index and schedule
</commit_message>
<xml_diff>
--- a/schedule_130.xlsx
+++ b/schedule_130.xlsx
@@ -129,10 +129,6 @@
 * Reproducible Research with R Markdown</t>
   </si>
   <si>
-    <t>Install programs on your personal computer [SlideDeck]()
-* Read Lab 1 overview</t>
-  </si>
-  <si>
     <t>Create Data Camp Account &amp; join class (Use emailed link!)</t>
   </si>
   <si>
@@ -148,6 +144,10 @@
     <t>Logistics 
 * Intro to R using Data Camp
 * How to get help</t>
+  </si>
+  <si>
+    <t>Install programs on your personal computer [[SlideDeck]]()
+* Read Lab 1 overview</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -933,11 +933,11 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>12</v>
@@ -960,7 +960,7 @@
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="32" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>13</v>
@@ -1084,10 +1084,10 @@
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="H8" s="43" t="s">
         <v>28</v>
@@ -1139,7 +1139,7 @@
         <v>17</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="7"/>
     </row>

</xml_diff>

<commit_message>
update theme, finalize schedule, ready to advertise
</commit_message>
<xml_diff>
--- a/schedule_130.xlsx
+++ b/schedule_130.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -50,24 +50,12 @@
     <t>eval</t>
   </si>
   <si>
-    <t>Exploratory Data Analysis</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
-    <t>Open work on EDA</t>
-  </si>
-  <si>
-    <t>Read the EDA Instructions</t>
-  </si>
-  <si>
     <t>Data Camp: Intro to R - Basics module 1 due by end of class</t>
   </si>
   <si>
-    <t>Lab 1</t>
-  </si>
-  <si>
     <t>Lab 2</t>
   </si>
   <si>
@@ -75,15 +63,6 @@
   </si>
   <si>
     <t>Lab 4</t>
-  </si>
-  <si>
-    <t>Proposal * Report</t>
-  </si>
-  <si>
-    <t>Peer Evaluation</t>
-  </si>
-  <si>
-    <t>Read Lab 2 overview</t>
   </si>
   <si>
     <t>Importing Data into R  
@@ -100,9 +79,6 @@
     <t>Data cleaning and aggregation</t>
   </si>
   <si>
-    <t>Read Lab 4 overview</t>
-  </si>
-  <si>
     <t>packages needed: tidyverse, rmarkdown, knitr, kable, kableExtra, gridExtra</t>
   </si>
   <si>
@@ -119,9 +95,6 @@
   </si>
   <si>
     <t>dplyr joins</t>
-  </si>
-  <si>
-    <t>Functions for Statistical Analyses</t>
   </si>
   <si>
     <t>R Studio suite of awesomeness
@@ -129,31 +102,35 @@
 * Reproducible Research with R Markdown</t>
   </si>
   <si>
-    <t>Create Data Camp Account &amp; join class (Use emailed link!)</t>
-  </si>
-  <si>
-    <t>Read Lab 5 overview</t>
-  </si>
-  <si>
-    <t>Lab 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baseball data? </t>
-  </si>
-  <si>
     <t>Logistics 
 * Intro to R using Data Camp
 * How to get help</t>
   </si>
   <si>
+    <t>Lab 1 (includes entire Data Camp Intro to R module)</t>
+  </si>
+  <si>
+    <t>Create Data Camp Account &amp; join class (Use emailed link!) * 
+Read [Day 1 intro](materials/day1-intro.html)</t>
+  </si>
+  <si>
+    <t>Read [Day 3 overview](materials/day3-import-and-factors.html) . *  Complete preparation steps.</t>
+  </si>
+  <si>
     <t>Install programs on your personal computer [[SlideDeck]]()
-* Read Lab 1 overview</t>
+* Read [Day 2 overview](materials/day2-rstudio.html)</t>
+  </si>
+  <si>
+    <t>Read [Week 3 overview](materials/day56-data-viz.html) . *  Complete preparation steps.</t>
+  </si>
+  <si>
+    <t>Read [Week 4 overview](materials/day78-data-manipulation.html) . *  Complete preparation steps.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -339,7 +316,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -362,12 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,9 +349,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -437,9 +405,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -475,6 +440,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -871,57 +839,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.08203125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1"/>
+    <col min="3" max="3" width="4.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.125" style="26" customWidth="1"/>
     <col min="7" max="7" width="23.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.58203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="29.625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="18"/>
+      <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -932,20 +900,20 @@
         <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="15"/>
+      <c r="D2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="35"/>
+      <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
         <f>B2+2</f>
@@ -955,22 +923,22 @@
         <f>TEXT(WEEKDAY(B3,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="40" t="s">
+      <c r="D3" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="H3" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -983,41 +951,31 @@
         <f>TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="29" t="s">
-        <v>19</v>
+      <c r="D4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="26" t="s">
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="21"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="5">
-        <f>B4+2</f>
-        <v>41516</v>
-      </c>
-      <c r="C5" s="6" t="str">
-        <f>TEXT(WEEKDAY(B5,1)+1, "ddd")</f>
-        <v>Thu</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="41"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>A4+1</f>
         <v>3</v>
@@ -1027,25 +985,25 @@
         <v>41521</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f t="shared" ref="C6:C11" si="0">TEXT(WEEKDAY(B6,1)+1, "ddd")</f>
+        <f t="shared" ref="C6:C9" si="0">TEXT(WEEKDAY(B6,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="29" t="s">
-        <v>24</v>
+      <c r="D6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="26" t="s">
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5">
         <f>B6+2</f>
@@ -1055,20 +1013,20 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="30"/>
+      <c r="D7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="42" t="s">
-        <v>26</v>
+      <c r="H7" s="38" t="s">
+        <v>18</v>
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" ref="A8:A10" si="1">A6+1</f>
+        <f t="shared" ref="A8" si="1">A6+1</f>
         <v>4</v>
       </c>
       <c r="B8" s="2">
@@ -1079,90 +1037,41 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D8" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="34" t="s">
-        <v>34</v>
+      <c r="D8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="26" t="s">
+        <v>30</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11">
+    <row r="9" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9">
         <f>B8+2</f>
         <v>41530</v>
       </c>
-      <c r="C9" s="12" t="str">
+      <c r="C9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D9" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B10" s="14">
-        <f>B8+7</f>
-        <v>41535</v>
-      </c>
-      <c r="C10" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Tue</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5">
-        <f>B10+2</f>
-        <v>41537</v>
-      </c>
-      <c r="C11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Thu</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="41"/>
-      <c r="I11" s="4"/>
+      <c r="D9" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>